<commit_message>
fixed luer-lock, added angle correspondence
</commit_message>
<xml_diff>
--- a/Turns vs Dispensed.xlsx
+++ b/Turns vs Dispensed.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9810" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Results with Angle Corresponden" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Number of Turns Counter Clockwise</t>
   </si>
@@ -40,18 +42,59 @@
   <si>
     <t>Standard Deviation</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Δ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Degree</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Δ Amount Dispensed (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µL)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -74,8 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -272,7 +316,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -314,7 +358,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Data!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -364,11 +408,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="5998032"/>
-        <c:axId val="5986064"/>
+        <c:axId val="-342273792"/>
+        <c:axId val="-342268896"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5998032"/>
+        <c:axId val="-342273792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -425,12 +469,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5986064"/>
+        <c:crossAx val="-342268896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5986064"/>
+        <c:axId val="-342268896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +531,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5998032"/>
+        <c:crossAx val="-342273792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -625,7 +669,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Data!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -722,7 +766,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -764,7 +808,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$12</c:f>
+              <c:f>Data!$D$2:$D$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -814,11 +858,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="5986608"/>
-        <c:axId val="5996400"/>
+        <c:axId val="-342269440"/>
+        <c:axId val="-226446464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="5986608"/>
+        <c:axId val="-342269440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -875,12 +919,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5996400"/>
+        <c:crossAx val="-226446464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="5996400"/>
+        <c:axId val="-226446464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -937,7 +981,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5986608"/>
+        <c:crossAx val="-342269440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1159,7 +1203,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1201,7 +1245,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$12</c:f>
+              <c:f>Data!$E$2:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1251,11 +1295,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="265364528"/>
-        <c:axId val="265367248"/>
+        <c:axId val="-96294496"/>
+        <c:axId val="-96293952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="265364528"/>
+        <c:axId val="-96294496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1343,12 +1387,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="265367248"/>
+        <c:crossAx val="-96293952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="265367248"/>
+        <c:axId val="-96293952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1436,7 +1480,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="265364528"/>
+        <c:crossAx val="-96294496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3248,6 +3292,54 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>490220</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>110491</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect l="27732" t="17073" r="29702" b="7236"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2105025" y="1466851"/>
+          <a:ext cx="4481195" cy="4358640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3511,9 +3603,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -3711,8 +3803,417 @@
         <v>2.5994364455994592E-2</v>
       </c>
     </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+10</f>
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <f>0.0082*(A3/360)*10^3</f>
+        <v>0.22777777777777777</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3+10</f>
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
+        <f t="shared" ref="B4:B38" si="0">0.0082*(A4/360)*10^3</f>
+        <v>0.45555555555555555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ref="A5:A38" si="1">A4+10</f>
+        <v>30</v>
+      </c>
+      <c r="B5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.68333333333333335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.91111111111111109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="B7" s="1">
+        <f t="shared" si="0"/>
+        <v>1.1388888888888888</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="B8" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3666666666666667</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B9" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5944444444444446</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="B10" s="1">
+        <f t="shared" si="0"/>
+        <v>1.8222222222222222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B11" s="1">
+        <f t="shared" si="0"/>
+        <v>2.0500000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="B12" s="1">
+        <f t="shared" si="0"/>
+        <v>2.2777777777777777</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="B13" s="1">
+        <f t="shared" si="0"/>
+        <v>2.505555555555556</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="B14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7333333333333334</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="B15" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9611111111111112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="B16" s="1">
+        <f t="shared" si="0"/>
+        <v>3.1888888888888891</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+      <c r="B17" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4166666666666674</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>3.6444444444444444</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="1"/>
+        <v>170</v>
+      </c>
+      <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8722222222222227</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1000000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>190</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3277777777777784</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>200</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="0"/>
+        <v>4.5555555555555554</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="0"/>
+        <v>4.7833333333333341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>5.011111111111112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>230</v>
+      </c>
+      <c r="B25" s="1">
+        <f t="shared" si="0"/>
+        <v>5.2388888888888889</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+      <c r="B26" s="1">
+        <f t="shared" si="0"/>
+        <v>5.4666666666666668</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>250</v>
+      </c>
+      <c r="B27" s="1">
+        <f t="shared" si="0"/>
+        <v>5.6944444444444446</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="B28" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9222222222222225</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>270</v>
+      </c>
+      <c r="B29" s="1">
+        <f t="shared" si="0"/>
+        <v>6.1500000000000012</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>280</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" si="0"/>
+        <v>6.3777777777777782</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>290</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="0"/>
+        <v>6.6055555555555561</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="0"/>
+        <v>6.8333333333333348</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>310</v>
+      </c>
+      <c r="B33" s="1">
+        <f t="shared" si="0"/>
+        <v>7.0611111111111118</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>320</v>
+      </c>
+      <c r="B34" s="1">
+        <f t="shared" si="0"/>
+        <v>7.2888888888888888</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
+      <c r="B35" s="1">
+        <f t="shared" si="0"/>
+        <v>7.5166666666666675</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>340</v>
+      </c>
+      <c r="B36" s="1">
+        <f t="shared" si="0"/>
+        <v>7.7444444444444454</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>350</v>
+      </c>
+      <c r="B37" s="1">
+        <f t="shared" si="0"/>
+        <v>7.9722222222222223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+      <c r="B38" s="1">
+        <f t="shared" si="0"/>
+        <v>8.2000000000000011</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
made a new luer-lock
</commit_message>
<xml_diff>
--- a/Turns vs Dispensed.xlsx
+++ b/Turns vs Dispensed.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Number of Turns Counter Clockwise</t>
   </si>
@@ -76,6 +76,9 @@
       </rPr>
       <t>µL)</t>
     </r>
+  </si>
+  <si>
+    <t>Nubmers</t>
   </si>
 </sst>
 </file>
@@ -408,11 +411,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-342273792"/>
-        <c:axId val="-342268896"/>
+        <c:axId val="1494956464"/>
+        <c:axId val="1494951568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-342273792"/>
+        <c:axId val="1494956464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -469,12 +472,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-342268896"/>
+        <c:crossAx val="1494951568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-342268896"/>
+        <c:axId val="1494951568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -531,7 +534,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-342273792"/>
+        <c:crossAx val="1494956464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -628,7 +631,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -858,11 +860,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-342269440"/>
-        <c:axId val="-226446464"/>
+        <c:axId val="1494952112"/>
+        <c:axId val="1494954288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-342269440"/>
+        <c:axId val="1494952112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -919,12 +921,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-226446464"/>
+        <c:crossAx val="1494954288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-226446464"/>
+        <c:axId val="1494954288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -981,7 +983,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-342269440"/>
+        <c:crossAx val="1494952112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1074,7 +1076,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1295,11 +1296,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-96294496"/>
-        <c:axId val="-96293952"/>
+        <c:axId val="1494954832"/>
+        <c:axId val="1494962448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-96294496"/>
+        <c:axId val="1494954832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,7 +1321,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1387,12 +1387,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-96293952"/>
+        <c:crossAx val="1494962448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-96293952"/>
+        <c:axId val="1494962448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1413,7 +1413,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1480,7 +1479,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-96294496"/>
+        <c:crossAx val="1494954832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1506,6 +1505,1014 @@
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Dispensed Amount</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22718572587185726"/>
+          <c:y val="0.10747346072186836"/>
+          <c:w val="0.60402270884022713"/>
+          <c:h val="0.79061571125265395"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Results with Angle Corresponden'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nubmers</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="17"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="18"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="19"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="20"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="21"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="22"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="23"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="24"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="25"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="26"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="27"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="28"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="29"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="30"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="31"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="32"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="33"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="34"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="35"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Results with Angle Corresponden'!$B:$B</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Results with Angle Corresponden'!$B$2:$B$1048576</c:f>
+              <c:strCache>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>0.00</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.37</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.59</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.82</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.05</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.28</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.51</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.73</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.96</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.19</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.42</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.64</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.87</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.10</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.33</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.56</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.78</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.01</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.47</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>5.69</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>5.92</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.15</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>6.38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6.61</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6.83</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.06</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7.29</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7.52</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7.74</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>7.97</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>8.20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Results with Angle Corresponden'!$C$2:$C$38</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Results with Angle Corresponden'!$C$3:$C$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent3"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent3"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1649,6 +2656,12 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="23">
+  <a:schemeClr val="accent3"/>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3193,6 +4206,530 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="260">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="0"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="0"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3299,13 +4836,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>490220</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>110491</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3319,8 +4856,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2105025" y="1466851"/>
-          <a:ext cx="4481195" cy="4358640"/>
+          <a:off x="3086100" y="1466849"/>
+          <a:ext cx="4067175" cy="4034791"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3335,6 +4872,36 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>123826</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3816,31 +5383,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+10</f>
         <v>10</v>
@@ -3849,8 +5425,11 @@
         <f>0.0082*(A3/360)*10^3</f>
         <v>0.22777777777777777</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+10</f>
         <v>20</v>
@@ -3859,8 +5438,11 @@
         <f t="shared" ref="B4:B38" si="0">0.0082*(A4/360)*10^3</f>
         <v>0.45555555555555555</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A38" si="1">A4+10</f>
         <v>30</v>
@@ -3869,8 +5451,11 @@
         <f t="shared" si="0"/>
         <v>0.68333333333333335</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -3879,8 +5464,11 @@
         <f t="shared" si="0"/>
         <v>0.91111111111111109</v>
       </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -3889,8 +5477,11 @@
         <f t="shared" si="0"/>
         <v>1.1388888888888888</v>
       </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -3899,8 +5490,11 @@
         <f t="shared" si="0"/>
         <v>1.3666666666666667</v>
       </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -3909,8 +5503,11 @@
         <f t="shared" si="0"/>
         <v>1.5944444444444446</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -3919,8 +5516,11 @@
         <f t="shared" si="0"/>
         <v>1.8222222222222222</v>
       </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -3929,8 +5529,11 @@
         <f t="shared" si="0"/>
         <v>2.0500000000000003</v>
       </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -3939,8 +5542,11 @@
         <f t="shared" si="0"/>
         <v>2.2777777777777777</v>
       </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -3949,8 +5555,11 @@
         <f t="shared" si="0"/>
         <v>2.505555555555556</v>
       </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -3959,8 +5568,11 @@
         <f t="shared" si="0"/>
         <v>2.7333333333333334</v>
       </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -3969,8 +5581,11 @@
         <f t="shared" si="0"/>
         <v>2.9611111111111112</v>
       </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="1"/>
         <v>140</v>
@@ -3979,8 +5594,11 @@
         <f t="shared" si="0"/>
         <v>3.1888888888888891</v>
       </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="1"/>
         <v>150</v>
@@ -3989,8 +5607,11 @@
         <f t="shared" si="0"/>
         <v>3.4166666666666674</v>
       </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="1"/>
         <v>160</v>
@@ -3999,8 +5620,11 @@
         <f t="shared" si="0"/>
         <v>3.6444444444444444</v>
       </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="1"/>
         <v>170</v>
@@ -4009,8 +5633,11 @@
         <f t="shared" si="0"/>
         <v>3.8722222222222227</v>
       </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>180</v>
@@ -4019,8 +5646,11 @@
         <f t="shared" si="0"/>
         <v>4.1000000000000005</v>
       </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>190</v>
@@ -4029,8 +5659,11 @@
         <f t="shared" si="0"/>
         <v>4.3277777777777784</v>
       </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>200</v>
@@ -4039,8 +5672,11 @@
         <f t="shared" si="0"/>
         <v>4.5555555555555554</v>
       </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>210</v>
@@ -4049,8 +5685,11 @@
         <f t="shared" si="0"/>
         <v>4.7833333333333341</v>
       </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="1"/>
         <v>220</v>
@@ -4059,8 +5698,11 @@
         <f t="shared" si="0"/>
         <v>5.011111111111112</v>
       </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="1"/>
         <v>230</v>
@@ -4069,8 +5711,11 @@
         <f t="shared" si="0"/>
         <v>5.2388888888888889</v>
       </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="1"/>
         <v>240</v>
@@ -4079,8 +5724,11 @@
         <f t="shared" si="0"/>
         <v>5.4666666666666668</v>
       </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="1"/>
         <v>250</v>
@@ -4089,8 +5737,11 @@
         <f t="shared" si="0"/>
         <v>5.6944444444444446</v>
       </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="1"/>
         <v>260</v>
@@ -4099,8 +5750,11 @@
         <f t="shared" si="0"/>
         <v>5.9222222222222225</v>
       </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="1"/>
         <v>270</v>
@@ -4109,8 +5763,11 @@
         <f t="shared" si="0"/>
         <v>6.1500000000000012</v>
       </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="1"/>
         <v>280</v>
@@ -4119,8 +5776,11 @@
         <f t="shared" si="0"/>
         <v>6.3777777777777782</v>
       </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="1"/>
         <v>290</v>
@@ -4129,8 +5789,11 @@
         <f t="shared" si="0"/>
         <v>6.6055555555555561</v>
       </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="1"/>
         <v>300</v>
@@ -4139,8 +5802,11 @@
         <f t="shared" si="0"/>
         <v>6.8333333333333348</v>
       </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="1"/>
         <v>310</v>
@@ -4149,8 +5815,11 @@
         <f t="shared" si="0"/>
         <v>7.0611111111111118</v>
       </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="1"/>
         <v>320</v>
@@ -4159,8 +5828,11 @@
         <f t="shared" si="0"/>
         <v>7.2888888888888888</v>
       </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="1"/>
         <v>330</v>
@@ -4169,8 +5841,11 @@
         <f t="shared" si="0"/>
         <v>7.5166666666666675</v>
       </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="1"/>
         <v>340</v>
@@ -4179,8 +5854,11 @@
         <f t="shared" si="0"/>
         <v>7.7444444444444454</v>
       </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="1"/>
         <v>350</v>
@@ -4189,8 +5867,11 @@
         <f t="shared" si="0"/>
         <v>7.9722222222222223</v>
       </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="1"/>
         <v>360</v>
@@ -4198,6 +5879,9 @@
       <c r="B38" s="1">
         <f t="shared" si="0"/>
         <v>8.2000000000000011</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 1uL Incuruments to turns
</commit_message>
<xml_diff>
--- a/Turns vs Dispensed.xlsx
+++ b/Turns vs Dispensed.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9810" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9810" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
     <sheet name="Angle Correspondence 45" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
   <si>
     <t>Number of Turns Counter Clockwise</t>
   </si>
@@ -122,9 +123,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,11 +415,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="453013680"/>
-        <c:axId val="453016944"/>
+        <c:axId val="1712213936"/>
+        <c:axId val="1712198704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="453013680"/>
+        <c:axId val="1712213936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -474,12 +476,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453016944"/>
+        <c:crossAx val="1712198704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="453016944"/>
+        <c:axId val="1712198704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,7 +538,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453013680"/>
+        <c:crossAx val="1712213936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -862,11 +864,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="580820336"/>
-        <c:axId val="580816528"/>
+        <c:axId val="1712210128"/>
+        <c:axId val="1712211760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="580820336"/>
+        <c:axId val="1712210128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -923,12 +925,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="580816528"/>
+        <c:crossAx val="1712211760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="580816528"/>
+        <c:axId val="1712211760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -985,7 +987,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="580820336"/>
+        <c:crossAx val="1712210128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1298,11 +1300,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="580820880"/>
-        <c:axId val="580817616"/>
+        <c:axId val="1712204688"/>
+        <c:axId val="1712211216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="580820880"/>
+        <c:axId val="1712204688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1389,12 +1391,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="580817616"/>
+        <c:crossAx val="1712211216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="580817616"/>
+        <c:axId val="1712211216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1481,7 +1483,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="580820880"/>
+        <c:crossAx val="1712204688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3325,7 +3327,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{78D7C0ED-F8E0-43DE-B6E8-BA41F316AE8D}" type="CELLRANGE">
+                    <a:fld id="{C0789A2D-BA63-404F-A2F0-E7CD519C8414}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3357,7 +3359,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CF92E413-3B4B-45E5-B79A-AB8584261A2C}" type="CELLRANGE">
+                    <a:fld id="{9A241262-9969-41D1-A6B8-ABA21D225677}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3389,7 +3391,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52A82D5A-2C0E-4C14-AF8D-F618FEF2FC08}" type="CELLRANGE">
+                    <a:fld id="{BAA459A5-F4C4-46AF-BA6A-C777512D4212}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3421,7 +3423,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC14F338-49AB-4029-AE3F-C18AEC7B5443}" type="CELLRANGE">
+                    <a:fld id="{79AACDC1-BDBC-4288-BB74-F9A0B60B2914}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3453,7 +3455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3AE29993-53C8-4C55-8B3A-C9610F85C0C4}" type="CELLRANGE">
+                    <a:fld id="{B9A7357F-70BB-4886-8D8C-C4C22400102D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3485,7 +3487,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EC6D5741-AD1D-4814-9A34-29E8E6265564}" type="CELLRANGE">
+                    <a:fld id="{73D9B98C-3773-474B-848C-5AE09BC79478}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3517,7 +3519,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B70AA10D-F8B0-437F-8301-DFB87BFC383E}" type="CELLRANGE">
+                    <a:fld id="{F1187986-D0BC-459F-9D71-0778F924F609}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3549,7 +3551,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{24511F3D-5775-49D3-BFA2-81DE2A739931}" type="CELLRANGE">
+                    <a:fld id="{CA9B4513-62E5-4F46-9B92-45F25354F0E5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3581,7 +3583,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1D7DCEC5-8523-42C1-A6AD-4CB185E761D3}" type="CELLRANGE">
+                    <a:fld id="{9EEA15C9-26C8-4068-8645-6A42D2BBAD56}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3613,7 +3615,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C9F6222-785E-4934-B510-5BFBF38F1F86}" type="CELLRANGE">
+                    <a:fld id="{2C00CF3D-1277-463B-9085-034BC4C770B4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3645,7 +3647,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F41E0A5-1C18-4EB1-852D-3D20C031E183}" type="CELLRANGE">
+                    <a:fld id="{83ACFD68-EAB3-4FD0-8048-76445803A039}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3677,7 +3679,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{453648F5-9C10-415D-8F93-707A94F10841}" type="CELLRANGE">
+                    <a:fld id="{6C098360-FDDC-4F2A-AA0A-E5A9F708F5C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3709,7 +3711,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1546F6C-0FCD-4393-AEB6-175C0EA064EF}" type="CELLRANGE">
+                    <a:fld id="{C0E1D4B0-D6D6-46D6-B1AA-75F05C34C594}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3741,7 +3743,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3F7156C7-293A-46DA-A6F3-619F3E24F06B}" type="CELLRANGE">
+                    <a:fld id="{A3714435-5DE1-41C9-8F0D-D787ADB6D3AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3773,7 +3775,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{29B0338A-2065-4616-91B0-507A6CC191A6}" type="CELLRANGE">
+                    <a:fld id="{1C90F435-15C4-4C6E-BABB-ED6B8E5476B3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3805,7 +3807,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{009AEE8F-98D7-4A00-8DA2-355FFAB357F1}" type="CELLRANGE">
+                    <a:fld id="{D73A8FF5-C62D-4F8D-B3D0-F1C4D046CFF8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3837,7 +3839,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2B9C3FDD-223C-4BA4-81AF-7DA4F305F0E3}" type="CELLRANGE">
+                    <a:fld id="{0764B131-FA52-49CA-930B-3B6D8759C560}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3869,7 +3871,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2679B470-FCA7-4E5A-AC68-2C8BAFA60E7F}" type="CELLRANGE">
+                    <a:fld id="{C1DFBA81-2433-4BEA-8EDC-569D023A5734}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3901,7 +3903,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{47159AD5-6B59-42F4-A749-B88A62EE01B1}" type="CELLRANGE">
+                    <a:fld id="{96673C72-7937-43D3-A54C-C6C539DC3964}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3933,7 +3935,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0C957389-A2BB-46D7-B703-66A350A6B67E}" type="CELLRANGE">
+                    <a:fld id="{844FEA28-AAEB-49E8-9454-29B79828A876}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3965,7 +3967,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A791B30E-12E6-49AB-AF6D-788737EFD980}" type="CELLRANGE">
+                    <a:fld id="{FC38ABF1-037B-4E3E-B74C-B2DBE88BADBF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3997,7 +3999,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5B17193C-D8ED-4197-AE1B-AF1F231DC8AA}" type="CELLRANGE">
+                    <a:fld id="{AC5942F5-E66E-417B-9E06-36750BCB253C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4029,7 +4031,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9992E0E3-FE6F-4989-BE4E-78535CBFEE74}" type="CELLRANGE">
+                    <a:fld id="{19B9B6CA-FD4C-48B3-B55A-0CBC69266C42}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4061,7 +4063,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8D7CAF8-88D4-4A44-A693-7AB0BBCC8CB2}" type="CELLRANGE">
+                    <a:fld id="{6FF50468-2446-422F-AA0F-0142E2028D10}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4093,7 +4095,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{388A79AB-BDFE-45E6-90DC-2152F7A328BB}" type="CELLRANGE">
+                    <a:fld id="{66125B26-B15C-4E5B-B30B-5D24DDACD943}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4125,7 +4127,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{529A2B56-6F58-412B-871B-933C9F4898DC}" type="CELLRANGE">
+                    <a:fld id="{D8EDCC39-8A0A-4053-895B-59602A062E28}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4157,7 +4159,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A94F8F3A-F4F0-46E8-94EA-2A84C150A0DC}" type="CELLRANGE">
+                    <a:fld id="{5D4C3B28-FF83-4128-A28C-5000CE27B7FE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4189,7 +4191,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90C6ACB8-E2A2-4904-AB92-59E172B716CE}" type="CELLRANGE">
+                    <a:fld id="{80496EFC-DB13-42E4-A67A-A2E80D987F6D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4221,7 +4223,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A59B6D93-52A3-4BC3-A3F6-D5C1C2949D33}" type="CELLRANGE">
+                    <a:fld id="{AB5C6B48-1DF1-4F65-A1D0-5CA5B0D43E8B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4253,7 +4255,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6AB7297A-3112-4524-926A-CCF4DE7E0885}" type="CELLRANGE">
+                    <a:fld id="{157AE2C1-D598-4CDF-97F5-0B310B55428C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4285,7 +4287,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{93BA17BC-08F0-4114-B93F-04AA82A0FCD4}" type="CELLRANGE">
+                    <a:fld id="{EEE9F305-D4B4-460C-8AD8-4875C224DB77}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4317,7 +4319,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{50590F51-96EA-4AE6-9BBD-06221E9F6056}" type="CELLRANGE">
+                    <a:fld id="{A6881831-EC3A-4377-BDD7-68351BF45CC5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4349,7 +4351,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9F2CDE01-E623-4B04-A177-A961B0FC4B57}" type="CELLRANGE">
+                    <a:fld id="{3CADBDD1-D2F8-44C2-8391-1F89CF41911D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4381,7 +4383,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED46C0FC-E679-4CA5-B916-357155AE72AC}" type="CELLRANGE">
+                    <a:fld id="{C22DD023-2ADD-4930-9F54-2C56CA5475F2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4413,7 +4415,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{118DBAFF-C21B-4A43-9A75-27832C60DA2F}" type="CELLRANGE">
+                    <a:fld id="{66283701-BEC8-4952-B690-57D89961B957}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4445,7 +4447,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB352D5B-1D8D-4730-B9E7-929228766BC4}" type="CELLRANGE">
+                    <a:fld id="{76A69916-8649-4D3B-A438-907FF441518B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4477,7 +4479,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2271C4A5-BC18-451B-98EE-49B90A8E0299}" type="CELLRANGE">
+                    <a:fld id="{3BA349EE-5423-4D12-8832-B2C817FBD3DF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5735,7 +5737,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40FC79A7-29A5-4AE9-9AF9-6C9D8CD15B04}" type="CELLRANGE">
+                    <a:fld id="{A1036C53-FD11-4B57-81B0-196129A68DC0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5767,7 +5769,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A11919FD-52A2-4C51-8862-F1AF1DFA8431}" type="CELLRANGE">
+                    <a:fld id="{792ECC02-D5CD-4DE2-AC87-8CC3A1AF0193}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5799,7 +5801,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6134F3CF-3742-4666-8405-70032FCB6E2D}" type="CELLRANGE">
+                    <a:fld id="{6FD9B62B-6420-44BF-BAB1-A551BA4DEE92}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5831,7 +5833,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{84B75F4E-6FC4-4770-A9CD-137EE3CE0979}" type="CELLRANGE">
+                    <a:fld id="{285E06F3-16F5-4AE8-89D5-7DAEBD541652}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5863,7 +5865,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BC355917-E2BE-4DA9-82D3-57C2BBDDE9B3}" type="CELLRANGE">
+                    <a:fld id="{705ED746-CD87-45E6-88A0-0482664EB464}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5895,7 +5897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{560B5ADD-DF67-4BBB-A119-CC8C4C052526}" type="CELLRANGE">
+                    <a:fld id="{A73B52E5-DBE7-4B2C-9E86-458E6D363059}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5927,7 +5929,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AE3591FE-7A88-43FD-8D18-DAA365E701C5}" type="CELLRANGE">
+                    <a:fld id="{E0748C43-9A28-4066-9AF6-877840FE41B5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5959,7 +5961,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{245B306F-2508-4C1B-9D5F-B5346C4961AF}" type="CELLRANGE">
+                    <a:fld id="{47E2C60C-F04A-4850-9A23-4494604D69A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5991,7 +5993,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{34BE2315-3591-4254-AE71-D88202EE4562}" type="CELLRANGE">
+                    <a:fld id="{9A8D4EB8-AF0A-49AE-BECB-B01855BFE610}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6023,7 +6025,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E29A1375-EE0B-4CA9-8B68-69A5EBF23310}" type="CELLRANGE">
+                    <a:fld id="{B4349AEC-6942-4A32-B547-9B69B1B8EF1E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6055,7 +6057,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{177A15DC-06F2-4FC2-8094-EC9AD5927F71}" type="CELLRANGE">
+                    <a:fld id="{5B8D34F2-BE4C-4236-973D-55C111E75DC5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6087,7 +6089,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E54192E3-9705-4C39-9DB5-468AA2A72A84}" type="CELLRANGE">
+                    <a:fld id="{381B3A7A-D370-413A-ACA4-E8B126896CAF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6119,7 +6121,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0BDAB284-F624-4D7F-9CF8-D26CBBF5567A}" type="CELLRANGE">
+                    <a:fld id="{752584F4-5B49-477A-9734-B01365795233}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6151,7 +6153,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B04855A9-EEA9-4A36-8E97-E33BD6BBE818}" type="CELLRANGE">
+                    <a:fld id="{172F5B04-D962-4EC1-A32A-02BD0E5086D5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6183,7 +6185,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{74082665-32CC-4396-8F78-A8B70E0B3F14}" type="CELLRANGE">
+                    <a:fld id="{BCC2B32E-BDD7-40AC-A827-7D32033DEFBA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6215,7 +6217,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1EFACEBB-B8B4-4943-9207-ECD73B8ADA81}" type="CELLRANGE">
+                    <a:fld id="{6D6BC2E1-36CB-43B2-9F9D-523500227D11}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6247,7 +6249,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{140D7DEE-BB09-4D00-A5C7-B64D2EECBB78}" type="CELLRANGE">
+                    <a:fld id="{FBB74DAA-FD6E-42C3-B8D7-7FA00CFF84BF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6279,7 +6281,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49C5AF7D-2818-413D-B88F-A4312E397782}" type="CELLRANGE">
+                    <a:fld id="{E2BFE66B-AD43-4753-B254-2EED8ABA20C7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6311,7 +6313,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1350DB13-557F-484F-9610-608E84BD4F4C}" type="CELLRANGE">
+                    <a:fld id="{317A4F65-FB6B-4A42-B80E-B1347754FFFA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6343,7 +6345,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DBAF2590-A96B-4E4E-B69E-9D1AAFBC7E13}" type="CELLRANGE">
+                    <a:fld id="{515EDEAB-CDA4-41EF-8AC3-DBCFA5181573}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6375,7 +6377,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4239C6D6-DB7B-4C72-ACBC-B782F0F65D39}" type="CELLRANGE">
+                    <a:fld id="{87002487-7760-4BC9-9ABB-40A613A2F79C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6407,7 +6409,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4BF97128-6263-4274-8B8E-23B9188A3D3D}" type="CELLRANGE">
+                    <a:fld id="{717E25E1-DD6A-4C8A-B184-42DAB4253362}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6439,7 +6441,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49868994-0125-4E7A-A2A0-8014483C894B}" type="CELLRANGE">
+                    <a:fld id="{DD991BA7-8D92-4B8E-801D-947526B45A67}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6471,7 +6473,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9637165B-AABE-4D1B-A2C3-1EA118F53BF6}" type="CELLRANGE">
+                    <a:fld id="{15D32A44-9AE1-44BB-920E-CAC13D617C37}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6503,7 +6505,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03E711EA-DC44-4986-8FAE-C48D6DF38155}" type="CELLRANGE">
+                    <a:fld id="{0E443EDF-A699-42C4-A37E-648F66A64BA3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6535,7 +6537,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{08032E18-4F87-4835-8B34-D57FECB57A25}" type="CELLRANGE">
+                    <a:fld id="{9CC417D3-FC60-4550-9F13-ED7D75FE070C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6567,7 +6569,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{36BD3FF3-855E-4F8C-AC95-030D7F2CB6B8}" type="CELLRANGE">
+                    <a:fld id="{C2011566-DCE0-48FA-BC8D-C6E4D20014B5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6599,7 +6601,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E5F84E8-02D9-4568-96AE-28A8EAA4DE18}" type="CELLRANGE">
+                    <a:fld id="{6A984700-9AB0-4BDD-8F76-FD22E1824737}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6631,7 +6633,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A8A0B3D8-370D-4725-98BC-39B82EC773BE}" type="CELLRANGE">
+                    <a:fld id="{D786A90C-D12C-43E9-B18C-A035F469C907}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6663,7 +6665,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B868D62A-425F-4803-BD66-7CCE8A11D2A4}" type="CELLRANGE">
+                    <a:fld id="{2B6B4233-9EB9-4690-9152-F97BC68B7F07}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6695,7 +6697,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CFDC3B6B-7716-4C2A-A7C1-272089C5BC3A}" type="CELLRANGE">
+                    <a:fld id="{A724606C-FF72-4C8F-95E3-40D5133C058F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6727,7 +6729,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B3962CB3-4B2A-49C3-8166-85E5D0327C85}" type="CELLRANGE">
+                    <a:fld id="{3867F9C8-A99C-4DB5-8876-16B50ABCBACF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6759,7 +6761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{532AB35C-D788-4EB8-8C2A-20BCAC2666E4}" type="CELLRANGE">
+                    <a:fld id="{007BC6EA-F183-4F2B-9B20-A12F2B1F4F73}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6791,7 +6793,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FCA70890-8C9C-4749-A3FE-23092EF28832}" type="CELLRANGE">
+                    <a:fld id="{5E663BF2-6F1E-4D4E-B0A5-FF53D076A0AB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6823,7 +6825,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{08D0CC0E-4FC6-4ADA-B345-A7E2603320DD}" type="CELLRANGE">
+                    <a:fld id="{24653691-E164-4A17-99F6-B0F68C51928B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6855,7 +6857,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F6EDA79-4C54-41FF-8586-9E486DCCF8F0}" type="CELLRANGE">
+                    <a:fld id="{56952789-CBCD-4A83-91EA-8B2C263A16A8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6887,7 +6889,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{42591093-8A34-477F-BBAD-33A9A1D24A14}" type="CELLRANGE">
+                    <a:fld id="{4CDB4040-5A2B-4DEF-A34A-2AA595B9D2A1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8145,7 +8147,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{88200713-7628-4B85-AB5D-8CEAA7452E0B}" type="CELLRANGE">
+                    <a:fld id="{A4817DB4-E67A-47F2-93EF-AB358CBC96FB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8177,7 +8179,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E070ABE1-A5CD-48AD-85F0-1B04B9F9CA1D}" type="CELLRANGE">
+                    <a:fld id="{B2FBB9B6-F008-4673-9B76-C86E111BAA7A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8209,7 +8211,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FDC61E0D-371A-42D4-853F-B149491DA4EB}" type="CELLRANGE">
+                    <a:fld id="{A0E5700A-494F-4239-BA57-2B68C5A39C68}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8241,7 +8243,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3E2E87C3-ABD2-4BB5-A12D-774F313294F2}" type="CELLRANGE">
+                    <a:fld id="{7B34395C-3358-4FD0-924A-377DAA3CB312}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8273,7 +8275,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C1638D2-E1BD-4280-9EF8-998AC8D974A0}" type="CELLRANGE">
+                    <a:fld id="{F4AB4F0B-5F01-43AC-B8A4-236F90736D15}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8305,7 +8307,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5BFF28B3-AA2D-4E7E-9E5E-1C9307727C26}" type="CELLRANGE">
+                    <a:fld id="{C51160D0-18AF-4427-9CDF-DEC0A0C9551D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8337,7 +8339,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{733F7C7A-78AF-4EB5-9133-76DE99516DCC}" type="CELLRANGE">
+                    <a:fld id="{BB4DD8B3-27E8-44D7-8A9B-8F8D748CDDD6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8369,7 +8371,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CB44DCD-553A-46C1-A6D8-F3319165797E}" type="CELLRANGE">
+                    <a:fld id="{526C5ED3-EFE5-417C-9B08-09604A6F5ED8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8401,7 +8403,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0312992F-390A-4299-A6DA-3BEE5BB48B30}" type="CELLRANGE">
+                    <a:fld id="{0971A318-BCC1-4397-B220-D12D6E4F63F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8433,7 +8435,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32645AFA-98AB-4FE3-9D83-9E7AEC8C9150}" type="CELLRANGE">
+                    <a:fld id="{4A6531DE-8D43-4927-9E09-32F2F0F066E9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8465,7 +8467,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F699D264-BEAC-4714-B060-CA4714B23AF6}" type="CELLRANGE">
+                    <a:fld id="{26158FAF-7097-4767-B17A-BC3BF745CDAF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8497,7 +8499,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B0D391C4-BA7E-43F2-A35D-59D37692D761}" type="CELLRANGE">
+                    <a:fld id="{107A7B01-B689-47F7-B031-B8F7726EC313}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8529,7 +8531,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC3DEEA3-5B18-4CEA-A8D4-7136623AF195}" type="CELLRANGE">
+                    <a:fld id="{F23165B5-70BD-4C49-9914-A808E677B469}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8561,7 +8563,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{13E0CAA1-0998-4331-AB45-4C940F6450AC}" type="CELLRANGE">
+                    <a:fld id="{DE5E3638-6473-4E9E-BE25-85483F9107CE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8593,7 +8595,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0034A778-705D-4442-AB54-B80A2E4841ED}" type="CELLRANGE">
+                    <a:fld id="{6D6E75DA-69EF-44CC-A95B-1224FDDBC2C3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8625,7 +8627,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F04D3FFA-7C08-4821-8B23-A30737CC9E6B}" type="CELLRANGE">
+                    <a:fld id="{2820C1DC-49F8-47D8-BB05-C0815FA50A86}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8657,7 +8659,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B7EA010C-5234-4ED5-8C81-E7AB8D8D979A}" type="CELLRANGE">
+                    <a:fld id="{5C171A2D-B51A-44CA-89CB-2ED5BD083ACF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8689,7 +8691,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{614E035A-A33A-4FAE-8D9F-F1CF46BC36BC}" type="CELLRANGE">
+                    <a:fld id="{F4630B23-FD37-4CD9-B07E-6787E6F9A333}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8721,7 +8723,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC10D50F-79CB-482F-A956-3A6F1FFAB6E2}" type="CELLRANGE">
+                    <a:fld id="{09F6EA22-9F5B-4B75-BD5C-91F8256EA425}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8753,7 +8755,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFDD81B8-541B-4291-85BE-7B533EA987B4}" type="CELLRANGE">
+                    <a:fld id="{F0181B5A-99DB-4636-85AA-10A55AB1EF7A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8785,7 +8787,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{08760BB4-16FE-4D38-9792-EAD2E257E9AE}" type="CELLRANGE">
+                    <a:fld id="{FF488E57-C880-4C61-BE73-06E8B85EE20B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8817,7 +8819,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{21584ACC-5854-43F3-8348-CB73BF0BC6AA}" type="CELLRANGE">
+                    <a:fld id="{1FFB1231-5E87-4477-841B-22E9EDF4DD59}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8849,7 +8851,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3638F9C6-1E5A-40C8-B47F-D3D82D1FCB92}" type="CELLRANGE">
+                    <a:fld id="{A04159EC-8269-4BC0-92F9-3A87251755EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8881,7 +8883,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89006C57-6C4B-4824-85CA-5AC5ECDE869D}" type="CELLRANGE">
+                    <a:fld id="{5546DC82-0DC2-46CA-A8D2-A2F15F54DE64}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8913,7 +8915,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2EDEC4AD-5A32-4751-A05D-002475E914D6}" type="CELLRANGE">
+                    <a:fld id="{066E24FF-E9A8-40E9-8AE2-67A96B3299D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8945,7 +8947,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3CEC53BD-87D4-49DB-8789-DA760B1787DE}" type="CELLRANGE">
+                    <a:fld id="{771BC2D0-3AB2-4978-A141-66D81B2B4C5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8977,7 +8979,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F3DF6EEA-0307-4B5A-9E89-92F1FF9AD766}" type="CELLRANGE">
+                    <a:fld id="{FBEE5114-D51A-4951-9167-CD9180A41D0E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9009,7 +9011,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{772206EB-C475-444D-9EC4-6E3E31BDDC73}" type="CELLRANGE">
+                    <a:fld id="{559CA7F8-8FFF-49BA-B611-81A003EA43AB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9041,7 +9043,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FE98DADA-7E33-453B-9923-1467CD004560}" type="CELLRANGE">
+                    <a:fld id="{812FFF2F-ABDE-4FAA-96CA-1D6064E7B8AE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9073,7 +9075,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25C02AFA-F8C5-43AF-9780-8492D92C92E4}" type="CELLRANGE">
+                    <a:fld id="{725BAF33-DB13-4586-8006-1B1D643DF097}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9105,7 +9107,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{471B37AE-2E44-407F-A2A7-79E5473EC693}" type="CELLRANGE">
+                    <a:fld id="{81765217-9ED0-4207-9D6D-9BBDA3B53FAA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9137,7 +9139,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C75D591A-2C35-473F-BD28-59E1DAB2B76F}" type="CELLRANGE">
+                    <a:fld id="{3C4282D5-D8BE-464C-B5F9-9CDDF2CC653A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9169,7 +9171,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{514903F5-7AB3-4975-8EC7-1330C210583D}" type="CELLRANGE">
+                    <a:fld id="{BD2D8FC6-B498-4583-B8A6-F94086B88A9D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9201,7 +9203,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D168F9F8-F4ED-4CF4-A3D8-7951EED9BE68}" type="CELLRANGE">
+                    <a:fld id="{12596F54-46B1-4338-BCBA-612D535AF534}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9233,7 +9235,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{68A7882E-E7CB-4F29-901F-51B21ADBA071}" type="CELLRANGE">
+                    <a:fld id="{A71D07DD-4F65-4DDE-9551-50E01FF94C2F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9265,7 +9267,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{023C574B-EC48-49A0-96DD-0E160B48905C}" type="CELLRANGE">
+                    <a:fld id="{01A735FC-D6A6-486C-A281-C44FF87A44F6}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9297,7 +9299,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DB51302A-579A-4D4B-A916-6DF764B62817}" type="CELLRANGE">
+                    <a:fld id="{17FB1428-B6F2-447A-AE30-8B13B83689A5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9850,12 +9852,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+              <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -9864,13 +9863,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Dispensed</a:t>
+              <a:t>Dispensed Chart</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Chart</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -9895,12 +9889,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -9919,18 +9910,27 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:shade val="45000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -9941,13 +9941,11 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:shade val="61000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -9958,13 +9956,11 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:shade val="76000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -9975,13 +9971,11 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:shade val="92000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -9992,13 +9986,11 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:tint val="93000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -10009,13 +10001,11 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:tint val="77000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -10026,13 +10016,11 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:tint val="62000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -10043,13 +10031,11 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:tint val="46000"/>
-                </a:schemeClr>
+                <a:schemeClr val="lt1"/>
               </a:solidFill>
               <a:ln w="19050">
                 <a:solidFill>
-                  <a:schemeClr val="lt1"/>
+                  <a:schemeClr val="accent3"/>
                 </a:solidFill>
               </a:ln>
               <a:effectLst/>
@@ -10070,12 +10056,9 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="accent3"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -10094,14 +10077,13 @@
             <c:showLeaderLines val="1"/>
             <c:leaderLines>
               <c:spPr>
-                <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:ln w="9525">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="35000"/>
-                      <a:lumOff val="65000"/>
+                    <a:schemeClr val="accent3">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:round/>
                 </a:ln>
                 <a:effectLst/>
               </c:spPr>
@@ -10190,7 +10172,7 @@
           <c:showLeaderLines val="1"/>
         </c:dLbls>
         <c:firstSliceAng val="0"/>
-        <c:holeSize val="75"/>
+        <c:holeSize val="50"/>
       </c:doughnutChart>
       <c:spPr>
         <a:noFill/>
@@ -10200,52 +10182,17 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr rtl="0">
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="accent3"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="accent3"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -10265,6 +10212,329 @@
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1500" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="7"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="60000"/>
+                      <a:lumOff val="40000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -10453,6 +10723,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -14078,86 +14388,81 @@
 </file>
 
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="260">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="0"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="0"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -14165,50 +14470,48 @@
       </a:solidFill>
       <a:ln>
         <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400">
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-      </a:ln>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -14216,35 +14519,44 @@
       <cs:styleClr val="auto"/>
     </cs:lnRef>
     <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="lt1"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
@@ -14256,7 +14568,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -14268,302 +14580,838 @@
     </cs:spPr>
   </cs:dataPointWireframe>
   <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="260">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="150" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="0"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <cs:styleClr val="0"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+      <a:effectLst>
+        <a:outerShdw dist="25400" dir="2700000" algn="tl" rotWithShape="0">
+          <a:schemeClr val="phClr"/>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="22225">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:dataTable>
   <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="35000"/>
+          <a:lumOff val="65000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:effectLst>
+        <a:glow rad="25400">
+          <a:schemeClr val="lt1"/>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:alpha val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:tint val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1500" b="1" kern="1200" cap="all" spc="100" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
   </cs:trendline>
   <cs:trendlineLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="0"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -14572,10 +15420,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
@@ -14584,14 +15429,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -14695,16 +15534,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:rowOff>24765</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14718,7 +15557,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3086100" y="1466849"/>
+          <a:off x="3838575" y="1323974"/>
           <a:ext cx="4067175" cy="4034791"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -14768,16 +15607,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>452436</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>233361</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>128587</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -14894,6 +15733,41 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>242887</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -15389,7 +16263,7 @@
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15911,7 +16785,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15923,10 +16797,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15968,11 +16845,11 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A38" si="0">A3+45</f>
+        <f t="shared" ref="A4:A10" si="0">A3+45</f>
         <v>90</v>
       </c>
       <c r="B4" s="1">
-        <f t="shared" ref="B4:B38" si="1">0.0082*(A4/360)*10^3</f>
+        <f t="shared" ref="B4:B10" si="1">0.0082*(A4/360)*10^3</f>
         <v>2.0500000000000003</v>
       </c>
       <c r="C4">
@@ -16145,4 +17022,150 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+45</f>
+        <v>45</v>
+      </c>
+      <c r="B3" s="2">
+        <f>0.0082*(A3/360)*10^3</f>
+        <v>1.0250000000000001</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A10" si="0">A3+45</f>
+        <v>90</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B10" si="1">0.0082*(A4/360)*10^3</f>
+        <v>2.0500000000000003</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="1"/>
+        <v>3.0750000000000006</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="1"/>
+        <v>4.1000000000000005</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>225</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="1"/>
+        <v>5.125</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="1"/>
+        <v>6.1500000000000012</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+      <c r="B9" s="2">
+        <f t="shared" si="1"/>
+        <v>7.1750000000000007</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="B10" s="2">
+        <f t="shared" si="1"/>
+        <v>8.2000000000000011</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>